<commit_message>
Added cave graphic to template and code
</commit_message>
<xml_diff>
--- a/ExcelLevels/tileTemplate.xlsx
+++ b/ExcelLevels/tileTemplate.xlsx
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="contentEnums">BoardEnums!$B$2:$B$7</definedName>
     <definedName name="entityEnums">BoardEnums!$E$2:$E$5</definedName>
-    <definedName name="graphicEnums">BoardEnums!$A$2:$A$10</definedName>
+    <definedName name="graphicEnums">BoardEnums!$A$2:$A$28</definedName>
     <definedName name="triggerStateEnums">BoardEnums!$C$2:$C$7</definedName>
     <definedName name="triggerTypeEnums">BoardEnums!$D$2:$D$4</definedName>
   </definedNames>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
   <si>
     <t>Graphic Enums</t>
   </si>
@@ -117,6 +117,51 @@
   </si>
   <si>
     <t>jump</t>
+  </si>
+  <si>
+    <t>cave_rock </t>
+  </si>
+  <si>
+    <t>cave_rockLight </t>
+  </si>
+  <si>
+    <t>cave_rockDark </t>
+  </si>
+  <si>
+    <t>cave_rockMossy </t>
+  </si>
+  <si>
+    <t>cave_rockWatery </t>
+  </si>
+  <si>
+    <t>cave_rockWaterPuddle </t>
+  </si>
+  <si>
+    <t>cave_rockBloody </t>
+  </si>
+  <si>
+    <t>cave_rockBloodPuddle </t>
+  </si>
+  <si>
+    <t>cave_rockLava </t>
+  </si>
+  <si>
+    <t>cave_sandstone </t>
+  </si>
+  <si>
+    <t>cave_sandstoneMossy </t>
+  </si>
+  <si>
+    <t>cave_sandstoneWatery </t>
+  </si>
+  <si>
+    <t>cave_lava</t>
+  </si>
+  <si>
+    <t>cave_rockHole </t>
+  </si>
+  <si>
+    <t>cave_rockBoulder</t>
   </si>
 </sst>
 </file>
@@ -1550,12 +1595,12 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -1672,38 +1717,103 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G17" s="2"/>
     </row>
-    <row r="23" spans="6:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
     </row>
   </sheetData>

</xml_diff>